<commit_message>
changing the code for the terms of reference
</commit_message>
<xml_diff>
--- a/version_python.xlsx
+++ b/version_python.xlsx
@@ -436,22 +436,22 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>version</t>
+          <t>Release version</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>release_date</t>
+          <t>Release date</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>download_link</t>
+          <t>Download</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>details_link</t>
+          <t>Release Notes</t>
         </is>
       </c>
     </row>

</xml_diff>